<commit_message>
melhorando a logica do balanco
</commit_message>
<xml_diff>
--- a/docs/buy_holder_sample.xlsx
+++ b/docs/buy_holder_sample.xlsx
@@ -15,8 +15,60 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>cristiano</author>
+  </authors>
+  <commentList>
+    <comment ref="O1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>balancoFroze</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>TotalPosicao</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G12" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>balancoPeso</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
   <si>
     <t>ITSA4</t>
   </si>
@@ -105,9 +157,6 @@
     <t>video</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
     <t>Liquido</t>
   </si>
   <si>
@@ -124,6 +173,15 @@
   </si>
   <si>
     <t>Fixo?</t>
+  </si>
+  <si>
+    <t>eggie3</t>
+  </si>
+  <si>
+    <t>insert into Balanco (IdCarteira,PesoPapel,FlagCongelado,IdPapel) values (3,1,'F',(select IdPapel from Papel where Codigo='</t>
+  </si>
+  <si>
+    <t>.SA'));</t>
   </si>
 </sst>
 </file>
@@ -134,7 +192,7 @@
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="#,##0_ ;\-#,##0\ "/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -163,6 +221,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -210,77 +275,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentagem" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="23">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3" tint="0.79998168889431442"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3" tint="0.79998168889431442"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -313,131 +308,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color theme="3" tint="0.79998168889431442"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor theme="3" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -737,17 +612,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E1:U18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C1:U22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T7" sqref="T7"/>
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="7" max="7" width="6.42578125" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" customWidth="1"/>
     <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7" customWidth="1"/>
     <col min="11" max="13" width="8" hidden="1" customWidth="1"/>
@@ -759,7 +634,7 @@
     <col min="21" max="21" width="12.140625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="4:21" x14ac:dyDescent="0.25">
       <c r="F1" t="s">
         <v>18</v>
       </c>
@@ -769,14 +644,14 @@
       <c r="H1" s="10"/>
       <c r="I1" s="10"/>
       <c r="N1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O1" s="1">
         <f>SUM(U6:U11)</f>
-        <v>5288</v>
-      </c>
-    </row>
-    <row r="2" spans="5:21" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="4:21" x14ac:dyDescent="0.25">
       <c r="F2" t="s">
         <v>5</v>
       </c>
@@ -787,16 +662,16 @@
       <c r="H2" s="11"/>
       <c r="I2" s="11"/>
       <c r="N2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O2" s="2">
         <f>G2-O1</f>
-        <v>16489</v>
-      </c>
-    </row>
-    <row r="3" spans="5:21" x14ac:dyDescent="0.25">
+        <v>21777</v>
+      </c>
+    </row>
+    <row r="3" spans="4:21" x14ac:dyDescent="0.25">
       <c r="F3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G3" s="11">
         <v>0</v>
@@ -804,7 +679,7 @@
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
     </row>
-    <row r="5" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="4:21" x14ac:dyDescent="0.25">
       <c r="F5" s="4" t="s">
         <v>10</v>
       </c>
@@ -846,13 +721,17 @@
         <v>15</v>
       </c>
       <c r="T5" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="U5" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="5:21" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="D6" t="str">
+        <f>CONCATENATE($C$21,F6,$C$22)</f>
+        <v>insert into Balanco (IdCarteira,PesoPapel,FlagCongelado,IdPapel) values (3,1,'F',(select IdPapel from Papel where Codigo='BRKM5.SA'));</v>
+      </c>
       <c r="E6" s="8" t="s">
         <v>19</v>
       </c>
@@ -864,14 +743,14 @@
       </c>
       <c r="H6" s="7">
         <f>G6/$G$12</f>
-        <v>0.25</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="I6" s="1">
         <v>44.51</v>
       </c>
       <c r="J6" s="3">
         <f>IF(T6="X",Q6,$O$2*H6/I6)</f>
-        <v>92.614019321500791</v>
+        <v>81.543473376769271</v>
       </c>
       <c r="K6" s="3">
         <f t="shared" ref="K6:K11" si="0">ROUNDDOWN(J6/100,0)*100</f>
@@ -895,7 +774,7 @@
       </c>
       <c r="P6" s="7">
         <f>O6/$O$12</f>
-        <v>0.19777827149522328</v>
+        <v>0.20736081993943628</v>
       </c>
       <c r="Q6">
         <v>100</v>
@@ -913,7 +792,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="D7" t="str">
+        <f t="shared" ref="D7:D11" si="6">CONCATENATE($C$21,F7,$C$22)</f>
+        <v>insert into Balanco (IdCarteira,PesoPapel,FlagCongelado,IdPapel) values (3,1,'F',(select IdPapel from Papel where Codigo='EMBR3.SA'));</v>
+      </c>
       <c r="E7" s="8" t="s">
         <v>20</v>
       </c>
@@ -924,15 +807,15 @@
         <v>1</v>
       </c>
       <c r="H7" s="7">
-        <f t="shared" ref="H7:H11" si="6">G7/$G$12</f>
-        <v>0.25</v>
+        <f t="shared" ref="H7:H11" si="7">G7/$G$12</f>
+        <v>0.16666666666666666</v>
       </c>
       <c r="I7" s="1">
         <v>22.68</v>
       </c>
       <c r="J7" s="3">
-        <f t="shared" ref="J7:J11" si="7">IF(T7="X",Q7,$O$2*H7/I7)</f>
-        <v>100</v>
+        <f>IF(T7="X",Q7,$O$2*H7/I7)</f>
+        <v>160.03086419753086</v>
       </c>
       <c r="K7" s="3">
         <f t="shared" si="0"/>
@@ -956,7 +839,7 @@
       </c>
       <c r="P7" s="7">
         <f t="shared" ref="P7:P11" si="9">O7/$O$12</f>
-        <v>0.10077760497667185</v>
+        <v>0.10566037735849057</v>
       </c>
       <c r="Q7">
         <v>100</v>
@@ -969,15 +852,16 @@
         <f t="shared" si="5"/>
         <v>0.10414657666345227</v>
       </c>
-      <c r="T7" t="s">
-        <v>29</v>
-      </c>
       <c r="U7" s="1">
         <f t="shared" ref="U7:U11" si="10">IF(T7="X",R7,0)</f>
-        <v>2268</v>
-      </c>
-    </row>
-    <row r="8" spans="5:21" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="D8" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into Balanco (IdCarteira,PesoPapel,FlagCongelado,IdPapel) values (3,1,'F',(select IdPapel from Papel where Codigo='GGBR4.SA'));</v>
+      </c>
       <c r="E8" s="9" t="s">
         <v>21</v>
       </c>
@@ -988,15 +872,15 @@
         <v>1</v>
       </c>
       <c r="H8" s="7">
-        <f t="shared" si="6"/>
-        <v>0.25</v>
+        <f t="shared" si="7"/>
+        <v>0.16666666666666666</v>
       </c>
       <c r="I8" s="1">
         <v>15.1</v>
       </c>
       <c r="J8" s="3">
-        <f t="shared" si="7"/>
-        <v>200</v>
+        <f t="shared" ref="J7:J11" si="11">IF(T8="X",Q8,$O$2*H8/I8)</f>
+        <v>240.36423841059604</v>
       </c>
       <c r="K8" s="3">
         <f t="shared" si="0"/>
@@ -1020,7 +904,7 @@
       </c>
       <c r="P8" s="7">
         <f t="shared" si="9"/>
-        <v>0.13419240168851365</v>
+        <v>0.14069415327276963</v>
       </c>
       <c r="Q8">
         <v>200</v>
@@ -1033,15 +917,16 @@
         <f t="shared" si="5"/>
         <v>0.13867842218854756</v>
       </c>
-      <c r="T8" t="s">
-        <v>29</v>
-      </c>
       <c r="U8" s="1">
         <f t="shared" si="10"/>
-        <v>3020</v>
-      </c>
-    </row>
-    <row r="9" spans="5:21" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="D9" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into Balanco (IdCarteira,PesoPapel,FlagCongelado,IdPapel) values (3,1,'F',(select IdPapel from Papel where Codigo='ITSA4.SA'));</v>
+      </c>
       <c r="E9" s="8" t="s">
         <v>19</v>
       </c>
@@ -1052,15 +937,15 @@
         <v>1</v>
       </c>
       <c r="H9" s="7">
-        <f t="shared" si="6"/>
-        <v>0.25</v>
+        <f t="shared" si="7"/>
+        <v>0.16666666666666666</v>
       </c>
       <c r="I9" s="1">
         <v>10.4</v>
       </c>
       <c r="J9" s="3">
-        <f t="shared" si="7"/>
-        <v>396.37019230769232</v>
+        <f t="shared" si="11"/>
+        <v>348.99038461538458</v>
       </c>
       <c r="K9" s="3">
         <f t="shared" si="0"/>
@@ -1072,19 +957,19 @@
       </c>
       <c r="M9" s="3">
         <f t="shared" si="8"/>
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="N9" s="3">
         <f t="shared" si="2"/>
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="O9" s="2">
         <f t="shared" si="3"/>
-        <v>4160</v>
+        <v>3120</v>
       </c>
       <c r="P9" s="7">
         <f t="shared" si="9"/>
-        <v>0.18484781159742281</v>
+        <v>0.14535290006988119</v>
       </c>
       <c r="Q9">
         <v>330</v>
@@ -1102,7 +987,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="D10" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into Balanco (IdCarteira,PesoPapel,FlagCongelado,IdPapel) values (3,1,'F',(select IdPapel from Papel where Codigo='VALE3.SA'));</v>
+      </c>
       <c r="E10" s="8" t="s">
         <v>19</v>
       </c>
@@ -1113,15 +1002,15 @@
         <v>1</v>
       </c>
       <c r="H10" s="7">
-        <f t="shared" si="6"/>
-        <v>0.25</v>
+        <f t="shared" si="7"/>
+        <v>0.16666666666666666</v>
       </c>
       <c r="I10" s="1">
         <v>51.52</v>
       </c>
       <c r="J10" s="3">
-        <f t="shared" si="7"/>
-        <v>80.012616459627324</v>
+        <f t="shared" si="11"/>
+        <v>70.448369565217391</v>
       </c>
       <c r="K10" s="3">
         <f t="shared" si="0"/>
@@ -1145,7 +1034,7 @@
       </c>
       <c r="P10" s="7">
         <f t="shared" si="9"/>
-        <v>0.22892690513219285</v>
+        <v>0.24001863498718845</v>
       </c>
       <c r="Q10">
         <v>100</v>
@@ -1163,7 +1052,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="D11" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into Balanco (IdCarteira,PesoPapel,FlagCongelado,IdPapel) values (3,1,'F',(select IdPapel from Papel where Codigo='WEGE3.SA'));</v>
+      </c>
       <c r="E11" s="8" t="s">
         <v>19</v>
       </c>
@@ -1174,15 +1067,15 @@
         <v>1</v>
       </c>
       <c r="H11" s="7">
-        <f t="shared" si="6"/>
-        <v>0.25</v>
+        <f t="shared" si="7"/>
+        <v>0.16666666666666666</v>
       </c>
       <c r="I11" s="1">
         <v>17.27</v>
       </c>
       <c r="J11" s="3">
-        <f t="shared" si="7"/>
-        <v>238.69426751592357</v>
+        <f t="shared" si="11"/>
+        <v>210.16213086276781</v>
       </c>
       <c r="K11" s="3">
         <f t="shared" si="0"/>
@@ -1206,7 +1099,7 @@
       </c>
       <c r="P11" s="7">
         <f t="shared" si="9"/>
-        <v>0.15347700510997556</v>
+        <v>0.16091311437223388</v>
       </c>
       <c r="Q11">
         <v>200</v>
@@ -1224,15 +1117,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="4:21" x14ac:dyDescent="0.25">
       <c r="F12" s="4"/>
       <c r="G12" s="4">
         <f>SUM(G6:G11)-T12</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H12" s="5">
         <f>SUM(H6:H11)</f>
-        <v>1.5</v>
+        <v>0.99999999999999989</v>
       </c>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
@@ -1242,7 +1135,7 @@
       <c r="N12" s="4"/>
       <c r="O12" s="6">
         <f>SUM(O6:O11)</f>
-        <v>22505</v>
+        <v>21465</v>
       </c>
       <c r="P12" s="6"/>
       <c r="Q12" s="4"/>
@@ -1252,13 +1145,13 @@
       </c>
       <c r="T12">
         <f>COUNTA(T6:T11)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="5:21" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="4:21" x14ac:dyDescent="0.25">
       <c r="J13" s="3"/>
     </row>
-    <row r="14" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="4:21" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
         <v>25</v>
       </c>
@@ -1266,7 +1159,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="4:21" x14ac:dyDescent="0.25">
       <c r="F15" t="s">
         <v>24</v>
       </c>
@@ -1274,7 +1167,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="4:21" x14ac:dyDescent="0.25">
       <c r="F16" t="s">
         <v>26</v>
       </c>
@@ -1282,7 +1175,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
       <c r="F17" t="s">
         <v>27</v>
       </c>
@@ -1290,12 +1183,30 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
       <c r="F18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G18">
         <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="F19" t="s">
+        <v>35</v>
+      </c>
+      <c r="G19">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1308,28 +1219,29 @@
     <mergeCell ref="G3:I3"/>
   </mergeCells>
   <conditionalFormatting sqref="Q6">
-    <cfRule type="cellIs" dxfId="9" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
       <formula>$N6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="7" operator="lessThan">
       <formula>$N6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q7:Q11">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
       <formula>$N7</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">
       <formula>$N7</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K11">
       <formula1>IF(K11&lt;&gt;Q11,1,2)</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
corrigindo ordenação dos campos
</commit_message>
<xml_diff>
--- a/docs/buy_holder_sample.xlsx
+++ b/docs/buy_holder_sample.xlsx
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
   <si>
     <t>ITSA4</t>
   </si>
@@ -182,6 +182,9 @@
   </si>
   <si>
     <t>.SA'));</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -615,8 +618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:U22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -648,7 +651,7 @@
       </c>
       <c r="O1" s="1">
         <f>SUM(U6:U11)</f>
-        <v>0</v>
+        <v>5371</v>
       </c>
     </row>
     <row r="2" spans="4:21" x14ac:dyDescent="0.25">
@@ -657,7 +660,7 @@
       </c>
       <c r="G2" s="11">
         <f>R12+G3</f>
-        <v>21777</v>
+        <v>24446.5</v>
       </c>
       <c r="H2" s="11"/>
       <c r="I2" s="11"/>
@@ -666,7 +669,7 @@
       </c>
       <c r="O2" s="2">
         <f>G2-O1</f>
-        <v>21777</v>
+        <v>19075.5</v>
       </c>
     </row>
     <row r="3" spans="4:21" x14ac:dyDescent="0.25">
@@ -674,7 +677,7 @@
         <v>29</v>
       </c>
       <c r="G3" s="11">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
@@ -743,18 +746,18 @@
       </c>
       <c r="H6" s="7">
         <f>G6/$G$12</f>
-        <v>0.16666666666666666</v>
+        <v>0.25</v>
       </c>
       <c r="I6" s="1">
-        <v>44.51</v>
+        <v>44.74</v>
       </c>
       <c r="J6" s="3">
         <f>IF(T6="X",Q6,$O$2*H6/I6)</f>
-        <v>81.543473376769271</v>
+        <v>106.59085829235583</v>
       </c>
       <c r="K6" s="3">
         <f t="shared" ref="K6:K11" si="0">ROUNDDOWN(J6/100,0)*100</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="L6" s="3">
         <f t="shared" ref="L6:L11" si="1">IF(K6=0,100,K6)</f>
@@ -770,22 +773,22 @@
       </c>
       <c r="O6" s="2">
         <f t="shared" ref="O6:O11" si="3">N6*I6</f>
-        <v>4451</v>
+        <v>4474</v>
       </c>
       <c r="P6" s="7">
         <f>O6/$O$12</f>
-        <v>0.20736081993943628</v>
+        <v>0.18354118805382344</v>
       </c>
       <c r="Q6">
         <v>100</v>
       </c>
       <c r="R6" s="2">
         <f t="shared" ref="R6:R11" si="4">Q6*I6</f>
-        <v>4451</v>
+        <v>4474</v>
       </c>
       <c r="S6" s="7">
         <f t="shared" ref="S6:S11" si="5">R6/$R$12</f>
-        <v>0.20438995270239244</v>
+        <v>0.20385938532340009</v>
       </c>
       <c r="U6" s="1">
         <f>IF(T6="X",R6,0)</f>
@@ -808,14 +811,14 @@
       </c>
       <c r="H7" s="7">
         <f t="shared" ref="H7:H11" si="7">G7/$G$12</f>
-        <v>0.16666666666666666</v>
+        <v>0.25</v>
       </c>
       <c r="I7" s="1">
-        <v>22.68</v>
+        <v>22.79</v>
       </c>
       <c r="J7" s="3">
         <f>IF(T7="X",Q7,$O$2*H7/I7)</f>
-        <v>160.03086419753086</v>
+        <v>100</v>
       </c>
       <c r="K7" s="3">
         <f t="shared" si="0"/>
@@ -835,26 +838,29 @@
       </c>
       <c r="O7" s="2">
         <f t="shared" si="3"/>
-        <v>2268</v>
+        <v>2279</v>
       </c>
       <c r="P7" s="7">
         <f t="shared" ref="P7:P11" si="9">O7/$O$12</f>
-        <v>0.10566037735849057</v>
+        <v>9.3493600262553336E-2</v>
       </c>
       <c r="Q7">
         <v>100</v>
       </c>
       <c r="R7" s="2">
         <f t="shared" si="4"/>
-        <v>2268</v>
+        <v>2279</v>
       </c>
       <c r="S7" s="7">
         <f t="shared" si="5"/>
-        <v>0.10414657666345227</v>
+        <v>0.10384343745016289</v>
+      </c>
+      <c r="T7" t="s">
+        <v>38</v>
       </c>
       <c r="U7" s="1">
         <f t="shared" ref="U7:U11" si="10">IF(T7="X",R7,0)</f>
-        <v>0</v>
+        <v>2279</v>
       </c>
     </row>
     <row r="8" spans="4:21" x14ac:dyDescent="0.25">
@@ -873,14 +879,14 @@
       </c>
       <c r="H8" s="7">
         <f t="shared" si="7"/>
-        <v>0.16666666666666666</v>
+        <v>0.25</v>
       </c>
       <c r="I8" s="1">
-        <v>15.1</v>
+        <v>15.46</v>
       </c>
       <c r="J8" s="3">
-        <f t="shared" ref="J7:J11" si="11">IF(T8="X",Q8,$O$2*H8/I8)</f>
-        <v>240.36423841059604</v>
+        <f t="shared" ref="J8:J11" si="11">IF(T8="X",Q8,$O$2*H8/I8)</f>
+        <v>200</v>
       </c>
       <c r="K8" s="3">
         <f t="shared" si="0"/>
@@ -900,26 +906,29 @@
       </c>
       <c r="O8" s="2">
         <f t="shared" si="3"/>
-        <v>3020</v>
+        <v>3092</v>
       </c>
       <c r="P8" s="7">
         <f t="shared" si="9"/>
-        <v>0.14069415327276963</v>
+        <v>0.12684607810961601</v>
       </c>
       <c r="Q8">
         <v>200</v>
       </c>
       <c r="R8" s="2">
         <f t="shared" si="4"/>
-        <v>3020</v>
+        <v>3092</v>
       </c>
       <c r="S8" s="7">
         <f t="shared" si="5"/>
-        <v>0.13867842218854756</v>
+        <v>0.14088806871255097</v>
+      </c>
+      <c r="T8" t="s">
+        <v>38</v>
       </c>
       <c r="U8" s="1">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>3092</v>
       </c>
     </row>
     <row r="9" spans="4:21" x14ac:dyDescent="0.25">
@@ -938,49 +947,49 @@
       </c>
       <c r="H9" s="7">
         <f t="shared" si="7"/>
-        <v>0.16666666666666666</v>
+        <v>0.25</v>
       </c>
       <c r="I9" s="1">
-        <v>10.4</v>
+        <v>10.35</v>
       </c>
       <c r="J9" s="3">
         <f t="shared" si="11"/>
-        <v>348.99038461538458</v>
+        <v>460.76086956521743</v>
       </c>
       <c r="K9" s="3">
         <f t="shared" si="0"/>
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="L9" s="3">
         <f t="shared" si="1"/>
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="M9" s="3">
         <f t="shared" si="8"/>
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="N9" s="3">
         <f t="shared" si="2"/>
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="O9" s="2">
         <f t="shared" si="3"/>
-        <v>3120</v>
+        <v>4140</v>
       </c>
       <c r="P9" s="7">
         <f t="shared" si="9"/>
-        <v>0.14535290006988119</v>
+        <v>0.16983918608467344</v>
       </c>
       <c r="Q9">
         <v>330</v>
       </c>
       <c r="R9" s="2">
         <f t="shared" si="4"/>
-        <v>3432</v>
+        <v>3415.5</v>
       </c>
       <c r="S9" s="7">
         <f t="shared" si="5"/>
-        <v>0.15759746521559442</v>
+        <v>0.15562846011892556</v>
       </c>
       <c r="U9" s="1">
         <f t="shared" si="10"/>
@@ -1003,14 +1012,14 @@
       </c>
       <c r="H10" s="7">
         <f t="shared" si="7"/>
-        <v>0.16666666666666666</v>
+        <v>0.25</v>
       </c>
       <c r="I10" s="1">
-        <v>51.52</v>
+        <v>52.76</v>
       </c>
       <c r="J10" s="3">
         <f t="shared" si="11"/>
-        <v>70.448369565217391</v>
+        <v>90.388078089461715</v>
       </c>
       <c r="K10" s="3">
         <f t="shared" si="0"/>
@@ -1030,22 +1039,22 @@
       </c>
       <c r="O10" s="2">
         <f t="shared" si="3"/>
-        <v>5152</v>
+        <v>5276</v>
       </c>
       <c r="P10" s="7">
         <f t="shared" si="9"/>
-        <v>0.24001863498718845</v>
+        <v>0.21644240236297999</v>
       </c>
       <c r="Q10">
         <v>100</v>
       </c>
       <c r="R10" s="2">
         <f t="shared" si="4"/>
-        <v>5152</v>
+        <v>5276</v>
       </c>
       <c r="S10" s="7">
         <f t="shared" si="5"/>
-        <v>0.23657987785278045</v>
+        <v>0.24040279771261933</v>
       </c>
       <c r="U10" s="1">
         <f t="shared" si="10"/>
@@ -1068,14 +1077,14 @@
       </c>
       <c r="H11" s="7">
         <f t="shared" si="7"/>
-        <v>0.16666666666666666</v>
+        <v>0.25</v>
       </c>
       <c r="I11" s="1">
-        <v>17.27</v>
+        <v>17.05</v>
       </c>
       <c r="J11" s="3">
         <f t="shared" si="11"/>
-        <v>210.16213086276781</v>
+        <v>279.69941348973606</v>
       </c>
       <c r="K11" s="3">
         <f t="shared" si="0"/>
@@ -1087,30 +1096,30 @@
       </c>
       <c r="M11" s="3">
         <f t="shared" si="8"/>
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="N11" s="3">
         <f t="shared" si="2"/>
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="O11" s="2">
         <f t="shared" si="3"/>
-        <v>3454</v>
+        <v>5115</v>
       </c>
       <c r="P11" s="7">
         <f t="shared" si="9"/>
-        <v>0.16091311437223388</v>
+        <v>0.2098375451263538</v>
       </c>
       <c r="Q11">
         <v>200</v>
       </c>
       <c r="R11" s="2">
         <f t="shared" si="4"/>
-        <v>3454</v>
+        <v>3410</v>
       </c>
       <c r="S11" s="7">
         <f t="shared" si="5"/>
-        <v>0.15860770537723287</v>
+        <v>0.15537785068234114</v>
       </c>
       <c r="U11" s="1">
         <f t="shared" si="10"/>
@@ -1121,11 +1130,11 @@
       <c r="F12" s="4"/>
       <c r="G12" s="4">
         <f>SUM(G6:G11)-T12</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H12" s="5">
         <f>SUM(H6:H11)</f>
-        <v>0.99999999999999989</v>
+        <v>1.5</v>
       </c>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
@@ -1135,17 +1144,17 @@
       <c r="N12" s="4"/>
       <c r="O12" s="6">
         <f>SUM(O6:O11)</f>
-        <v>21465</v>
+        <v>24376</v>
       </c>
       <c r="P12" s="6"/>
       <c r="Q12" s="4"/>
       <c r="R12" s="6">
         <f>SUM(R6:R11)</f>
-        <v>21777</v>
+        <v>21946.5</v>
       </c>
       <c r="T12">
         <f>COUNTA(T6:T11)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="4:21" x14ac:dyDescent="0.25">

</xml_diff>